<commit_message>
update route and add spinner
</commit_message>
<xml_diff>
--- a/TCH.BackendApi/Uploads/temp-order.xlsx
+++ b/TCH.BackendApi/Uploads/temp-order.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>Báo cáo bán hàng của tất cả cửa hàng</t>
   </si>
   <si>
-    <t>Ngày báo cáo: 06/07/2022</t>
+    <t>Ngày báo cáo: 06/10/2022</t>
   </si>
   <si>
     <t>STT</t>
@@ -140,22 +140,25 @@
     <t>HP Trần Quang Khải</t>
   </si>
   <si>
+    <t>ORDER.N00-7</t>
+  </si>
+  <si>
+    <t>06/02/2022</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -05/05/2022</t>
+  </si>
+  <si>
+    <t>HP Trần Phú</t>
+  </si>
+  <si>
     <t>ORDER.N00-10</t>
   </si>
   <si>
-    <t>06/02/2022</t>
-  </si>
-  <si>
     <t>HP Aeon Mall Lê Chân</t>
   </si>
   <si>
-    <t>ORDER.N00-7</t>
-  </si>
-  <si>
-    <t>Đơn hàng ngày -05/05/2022</t>
-  </si>
-  <si>
-    <t>HP Trần Phú</t>
+    <t>Đơn hàng ngày -09/01/2022</t>
   </si>
   <si>
     <t>ORDER.N00-22</t>
@@ -164,9 +167,6 @@
     <t>Đơn hàng ngày -01/01/2022</t>
   </si>
   <si>
-    <t>Đơn hàng ngày -09/01/2022</t>
-  </si>
-  <si>
     <t>ORDER.N00-27</t>
   </si>
   <si>
@@ -200,10 +200,16 @@
     <t>06/04/2022</t>
   </si>
   <si>
+    <t>Đơn hàng ngày -11/05/2022</t>
+  </si>
+  <si>
     <t>Đơn hàng ngày -02/07/2022</t>
   </si>
   <si>
-    <t>Đơn hàng ngày -11/05/2022</t>
+    <t>ORDER.N00-1</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -05/14/2022</t>
   </si>
   <si>
     <t>ORDER.N00-6</t>
@@ -215,48 +221,42 @@
     <t>888.000.000</t>
   </si>
   <si>
-    <t>ORDER.N00-1</t>
-  </si>
-  <si>
-    <t>Đơn hàng ngày -05/14/2022</t>
-  </si>
-  <si>
     <t>Đơn hàng ngày -11/15/2022</t>
   </si>
   <si>
+    <t>ORDER.N00-19</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -03/20/2022</t>
+  </si>
+  <si>
+    <t>ORDER.N00-4</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -09/07/2022</t>
+  </si>
+  <si>
     <t>ORDER.N00-24</t>
   </si>
   <si>
     <t>Đơn hàng ngày -11/13/2022</t>
   </si>
   <si>
-    <t>ORDER.N00-19</t>
-  </si>
-  <si>
-    <t>Đơn hàng ngày -03/20/2022</t>
-  </si>
-  <si>
-    <t>ORDER.N00-4</t>
-  </si>
-  <si>
-    <t>Đơn hàng ngày -09/07/2022</t>
+    <t>06/05/2022</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -08/20/2022</t>
   </si>
   <si>
     <t>ORDER.N00-21</t>
   </si>
   <si>
-    <t>06/05/2022</t>
-  </si>
-  <si>
     <t>Đơn hàng ngày -03/11/2022</t>
   </si>
   <si>
     <t>828.000.000</t>
   </si>
   <si>
-    <t>Đơn hàng ngày -08/20/2022</t>
-  </si>
-  <si>
     <t>Đơn hàng ngày -08/18/2022</t>
   </si>
   <si>
@@ -320,10 +320,163 @@
     <t>58.000</t>
   </si>
   <si>
+    <t>ORDER.N052-8</t>
+  </si>
+  <si>
+    <t>linhh</t>
+  </si>
+  <si>
+    <t>06/08/2022</t>
+  </si>
+  <si>
+    <t>Tiền mặt</t>
+  </si>
+  <si>
+    <t>108.000</t>
+  </si>
+  <si>
+    <t>-10.000</t>
+  </si>
+  <si>
+    <t>118.000</t>
+  </si>
+  <si>
+    <t>ORDER.N056-8</t>
+  </si>
+  <si>
+    <t>80.000</t>
+  </si>
+  <si>
+    <t>2.000</t>
+  </si>
+  <si>
+    <t>78.000</t>
+  </si>
+  <si>
+    <t>06/09/2022</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -10/19/2022</t>
+  </si>
+  <si>
+    <t>468.000.000</t>
+  </si>
+  <si>
+    <t>ORDER.N00-15</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -01/04/2022</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -03/15/2022</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -01/03/2022</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -11/21/2022</t>
+  </si>
+  <si>
+    <t>ORDER.N037-9</t>
+  </si>
+  <si>
+    <t>100.000</t>
+  </si>
+  <si>
+    <t>20.000</t>
+  </si>
+  <si>
+    <t>ORDER.N038-9</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>06/10/2022</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -04/12/2022</t>
+  </si>
+  <si>
+    <t>624.000.000</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -02/10/2022</t>
+  </si>
+  <si>
+    <t>Đơn hàng ngày -07/04/2022</t>
+  </si>
+  <si>
+    <t>ORDER.N019-10</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>39.000</t>
+  </si>
+  <si>
+    <t>ORDER.N010-10</t>
+  </si>
+  <si>
+    <t>700.000</t>
+  </si>
+  <si>
+    <t>24.000</t>
+  </si>
+  <si>
+    <t>676.000</t>
+  </si>
+  <si>
+    <t>ORDER.N014-10</t>
+  </si>
+  <si>
+    <t>4.000.000</t>
+  </si>
+  <si>
+    <t>3.900.000</t>
+  </si>
+  <si>
+    <t>ORDER.N016-10</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>6.000.000</t>
+  </si>
+  <si>
+    <t>300.000</t>
+  </si>
+  <si>
+    <t>5.700.000</t>
+  </si>
+  <si>
+    <t>Ship đồ</t>
+  </si>
+  <si>
+    <t>ORDER.N026-10</t>
+  </si>
+  <si>
+    <t>ORDER.N027-10</t>
+  </si>
+  <si>
+    <t>ph</t>
+  </si>
+  <si>
+    <t>50.000</t>
+  </si>
+  <si>
+    <t>1.000</t>
+  </si>
+  <si>
+    <t>49.000</t>
+  </si>
+  <si>
     <t>Doanh thu bán hàng</t>
   </si>
   <si>
-    <t>8.352.058.000</t>
+    <t>11.572.554.000</t>
   </si>
 </sst>
 </file>
@@ -441,7 +594,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -800,25 +953,25 @@
         <v>42</v>
       </c>
       <c r="C11" s="0">
-        <v>670</v>
+        <v>57</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>43</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>24</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>26</v>
@@ -827,7 +980,7 @@
         <v>26</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="N11" s="0" t="s">
         <v>26</v>
@@ -836,10 +989,10 @@
         <v>26</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
@@ -847,22 +1000,22 @@
         <v>6</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="0">
-        <v>57</v>
+        <v>670</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>43</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>24</v>
@@ -877,7 +1030,7 @@
         <v>26</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="N12" s="0" t="s">
         <v>26</v>
@@ -886,10 +1039,10 @@
         <v>26</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
@@ -897,10 +1050,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0">
-        <v>712</v>
+        <v>780</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>33</v>
@@ -912,7 +1065,7 @@
         <v>34</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>24</v>
@@ -947,10 +1100,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0">
-        <v>780</v>
+        <v>712</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>33</v>
@@ -1118,7 +1271,7 @@
         <v>24</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K17" s="0" t="s">
         <v>26</v>
@@ -1168,7 +1321,7 @@
         <v>24</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K18" s="0" t="s">
         <v>26</v>
@@ -1247,19 +1400,19 @@
         <v>14</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="0">
-        <v>947</v>
+        <v>812</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>61</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>62</v>
@@ -1268,7 +1421,7 @@
         <v>24</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K20" s="0" t="s">
         <v>26</v>
@@ -1277,7 +1430,7 @@
         <v>26</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="N20" s="0" t="s">
         <v>26</v>
@@ -1286,10 +1439,10 @@
         <v>26</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q20" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
@@ -1297,19 +1450,19 @@
         <v>15</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C21" s="0">
-        <v>812</v>
+        <v>947</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>61</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>63</v>
@@ -1318,7 +1471,7 @@
         <v>24</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>26</v>
@@ -1327,7 +1480,7 @@
         <v>26</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="N21" s="0" t="s">
         <v>26</v>
@@ -1336,10 +1489,10 @@
         <v>26</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22">
@@ -1350,16 +1503,16 @@
         <v>64</v>
       </c>
       <c r="C22" s="0">
-        <v>531</v>
+        <v>144</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>61</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>65</v>
@@ -1368,7 +1521,7 @@
         <v>24</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K22" s="0" t="s">
         <v>26</v>
@@ -1377,7 +1530,7 @@
         <v>26</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="N22" s="0" t="s">
         <v>26</v>
@@ -1386,10 +1539,10 @@
         <v>26</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
@@ -1397,38 +1550,38 @@
         <v>17</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="0">
-        <v>144</v>
+        <v>531</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>61</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G23" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="H23" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="N23" s="0" t="s">
         <v>26</v>
       </c>
@@ -1436,10 +1589,10 @@
         <v>26</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="Q23" s="0" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24">
@@ -1447,7 +1600,7 @@
         <v>18</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C24" s="0">
         <v>800</v>
@@ -1468,7 +1621,7 @@
         <v>24</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K24" s="0" t="s">
         <v>26</v>
@@ -1500,7 +1653,7 @@
         <v>70</v>
       </c>
       <c r="C25" s="0">
-        <v>758</v>
+        <v>634</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>33</v>
@@ -1518,7 +1671,7 @@
         <v>24</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="K25" s="0" t="s">
         <v>26</v>
@@ -1550,7 +1703,7 @@
         <v>72</v>
       </c>
       <c r="C26" s="0">
-        <v>634</v>
+        <v>266</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>33</v>
@@ -1600,7 +1753,7 @@
         <v>74</v>
       </c>
       <c r="C27" s="0">
-        <v>266</v>
+        <v>758</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>33</v>
@@ -1618,7 +1771,7 @@
         <v>24</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="K27" s="0" t="s">
         <v>26</v>
@@ -1647,28 +1800,28 @@
         <v>22</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="C28" s="0">
-        <v>181</v>
+        <v>657</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>24</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K28" s="0" t="s">
         <v>26</v>
@@ -1677,7 +1830,7 @@
         <v>26</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="N28" s="0" t="s">
         <v>26</v>
@@ -1686,10 +1839,10 @@
         <v>26</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29">
@@ -1697,38 +1850,38 @@
         <v>23</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="C29" s="0">
-        <v>657</v>
+        <v>181</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>20</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>22</v>
       </c>
       <c r="G29" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M29" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H29" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J29" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="K29" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L29" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M29" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="N29" s="0" t="s">
         <v>26</v>
       </c>
@@ -1736,10 +1889,10 @@
         <v>26</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="Q29" s="0" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30">
@@ -1747,7 +1900,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C30" s="0">
         <v>417</v>
@@ -1756,7 +1909,7 @@
         <v>20</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>22</v>
@@ -1897,7 +2050,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="0">
         <v>213</v>
@@ -1918,7 +2071,7 @@
         <v>24</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K33" s="0" t="s">
         <v>26</v>
@@ -1968,7 +2121,7 @@
         <v>24</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K34" s="0" t="s">
         <v>26</v>
@@ -1997,7 +2150,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" s="0">
         <v>43</v>
@@ -2018,7 +2171,7 @@
         <v>24</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K35" s="0" t="s">
         <v>26</v>
@@ -2047,7 +2200,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C36" s="0">
         <v>854</v>
@@ -2142,35 +2295,976 @@
         <v>101</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>32</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="0">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M38" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N38" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="O38" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P38" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q38" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="39">
-      <c r="A39" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="6" t="s">
+      <c r="A39" s="0">
+        <v>33</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="0">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>103</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M39" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="N39" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="O39" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P39" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q39" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>34</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="0">
+        <v>835</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M40" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="N40" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O40" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P40" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q40" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>35</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="0">
+        <v>665</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N41" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O41" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P41" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q41" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>36</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="0">
+        <v>965</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M42" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="N42" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O42" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P42" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q42" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>37</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="0">
+        <v>312</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N43" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O43" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P43" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q43" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>38</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="0">
+        <v>326</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M44" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N44" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O44" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P44" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q44" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>39</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="0">
+        <v>1</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L45" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M45" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="N45" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="O45" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P45" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q45" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>40</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="0">
+        <v>5</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L46" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M46" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="N46" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O46" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P46" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q46" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>41</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="0">
+        <v>863</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K47" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L47" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M47" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="N47" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O47" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P47" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q47" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>42</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="0">
+        <v>37</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L48" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M48" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="N48" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O48" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P48" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q48" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>43</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="0">
+        <v>732</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K49" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L49" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M49" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N49" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O49" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P49" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q49" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>44</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="0">
+        <v>2</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L50" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M50" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="N50" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O50" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P50" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q50" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>45</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="0">
+        <v>12</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K51" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L51" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M51" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="N51" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="O51" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P51" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q51" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>46</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" s="0">
+        <v>1</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K52" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L52" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M52" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="N52" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="O52" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P52" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q52" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>47</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="0">
+        <v>2</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L53" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M53" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="N53" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="O53" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P53" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q53" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>48</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="0">
+        <v>2</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L54" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M54" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="N54" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="O54" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="P54" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q54" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>49</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" s="0">
+        <v>2</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L55" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M55" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="N55" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O55" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P55" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q55" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>50</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C56" s="0">
+        <v>2</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L56" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M56" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="N56" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="O56" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P56" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q56" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A39:P39"/>
-    <mergeCell ref="Q39:Q39"/>
+    <mergeCell ref="A58:P58"/>
+    <mergeCell ref="Q58:Q58"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>